<commit_message>
[FIX]Correcion de algunos errores al rellenar excel
</commit_message>
<xml_diff>
--- a/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -882,7 +882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="95" zoomScaleNormal="95">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A645" ySplit="11"/>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>data_size=41</t>
+          <t>description=Predefined data item for storing the configuration ID</t>
         </is>
       </c>
     </row>
@@ -1432,18 +1432,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TestData_07</t>
+          <t>TestData_08</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12345</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
+        <v>12346</v>
+      </c>
+      <c r="C18" t="n">
+        <v>87</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1455,21 +1458,47 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>description=- Component: Test
-- REPROG info: To be evaluated.</t>
-        </is>
+          <t>HOLA</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>JULIO</t>
+        </is>
+      </c>
+      <c r="R18" t="n">
+        <v>8</v>
+      </c>
+      <c r="S18" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TestData_08</t>
+          <t>TestData_09</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12346</v>
-      </c>
-      <c r="I19" t="inlineStr">
+        <v>12347</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1479,23 +1508,59 @@
           <t>ee_range</t>
         </is>
       </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>BB96</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>description=- Component: TST Data
-- REPROG info: undefined</t>
-        </is>
+          <t>ADIOS</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>RUBEN</t>
+        </is>
+      </c>
+      <c r="R19" t="n">
+        <v>7</v>
+      </c>
+      <c r="S19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TestData_09</t>
+          <t>TestData_10</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12347</v>
-      </c>
-      <c r="G20" t="inlineStr">
+        <v>12348</v>
+      </c>
+      <c r="C20" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1505,21 +1570,57 @@
           <t>ee_range</t>
         </is>
       </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>BB75</t>
+        </is>
+      </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>description=- Component: TST Data
-- REPROG info: tbd</t>
-        </is>
+          <t>:(</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>JULIO Y RUBEN</t>
+        </is>
+      </c>
+      <c r="R20" t="n">
+        <v>6</v>
+      </c>
+      <c r="S20" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TestData_10</t>
+          <t>TestData_11</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12348</v>
+        <v>12349</v>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1533,29 +1634,37 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>ee_range</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>description=- Component: TST
-- REPROG info: t.b.d</t>
-        </is>
+          <t>datablock</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>BB89</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>JEJ</t>
+        </is>
+      </c>
+      <c r="R21" t="n">
+        <v>5</v>
+      </c>
+      <c r="S21" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TestData_11</t>
+          <t>DUMMY_TestModuleCnt</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>12349</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>31416</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1564,24 +1673,27 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>ee_range</t>
+          <t>ee_erase</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>description=- Component: TST
-- REPROG info: use case REPROG must be set</t>
+          <t>description=- Component: DUMMY
+- REPROG info: use case REPROG must not be set (data must not be changed after reprogramming)!
+Sometimes the description is longer than two rows.
+Other times, there are more than three.
+In this case, it is one more than four. And could be more.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TestData_11</t>
+          <t>ASDFClockTower</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12349</v>
+        <v>111255</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1590,56 +1702,57 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>ee_range</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>DUMMY_TestModuleCnt</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>31416</v>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>ee_erase</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>ASDFClockTower</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>111255</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
           <t>ee_datablock</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>description=- Component: ASDF
 - REPROG info: use case REPROG must not be set.
 - REPROG info: In certain cases there are two comments of this type.
 There are also strings up to 160 characters per row, only on description fields and usually is not only one row. Like this example but a little bit longer.</t>
         </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TestData_07</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C24" t="n">
+        <v>91</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="S24" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX]Logs corregidos, son ordenados de forma tabular
</commit_message>
<xml_diff>
--- a/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1469,9 +1469,6 @@
           <t>JULIO</t>
         </is>
       </c>
-      <c r="R18" t="n">
-        <v>8</v>
-      </c>
       <c r="S18" t="n">
         <v>5</v>
       </c>
@@ -1521,11 +1518,6 @@
       <c r="P19" t="n">
         <v>6</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>RUBEN</t>
-        </is>
-      </c>
       <c r="R19" t="n">
         <v>7</v>
       </c>
@@ -1580,9 +1572,6 @@
           <t>:(</t>
         </is>
       </c>
-      <c r="P20" t="n">
-        <v>5</v>
-      </c>
       <c r="Q20" t="inlineStr">
         <is>
           <t>JULIO Y RUBEN</t>
@@ -1603,9 +1592,6 @@
       </c>
       <c r="B21" t="n">
         <v>12349</v>
-      </c>
-      <c r="C21" t="n">
-        <v>5</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1749,6 +1735,12 @@
       <c r="M24" t="inlineStr">
         <is>
           <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>description=- Component: Test
+- REPROG info: To be evaluated.</t>
         </is>
       </c>
       <c r="S24" t="n">

</xml_diff>

<commit_message>
[fix]Correcciones del user manual
</commit_message>
<xml_diff>
--- a/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1432,21 +1432,18 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TestData_08</t>
+          <t>TestData_07</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12346</v>
-      </c>
-      <c r="C18" t="n">
-        <v>87</v>
-      </c>
-      <c r="E18" t="inlineStr">
+        <v>12345</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1458,211 +1455,150 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>HOLA</t>
-        </is>
-      </c>
-      <c r="P18" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>JULIO</t>
-        </is>
-      </c>
-      <c r="S18" t="n">
-        <v>5</v>
+          <t>description=- Component: Test
+- REPROG info: To be evaluated.</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TestData_09</t>
+          <t>TestData_08</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12347</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" t="inlineStr">
+        <v>12346</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M19" t="inlineStr">
         <is>
           <t>ee_range</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>BB96</t>
-        </is>
-      </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>ADIOS</t>
-        </is>
-      </c>
-      <c r="P19" t="n">
-        <v>6</v>
-      </c>
-      <c r="R19" t="n">
-        <v>7</v>
-      </c>
-      <c r="S19" t="n">
-        <v>3</v>
+          <t>description=- Component: TST Data
+- REPROG info: undefined</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TestData_10</t>
+          <t>TestData_09</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12348</v>
-      </c>
-      <c r="C20" t="n">
-        <v>9</v>
-      </c>
-      <c r="D20" t="inlineStr">
+        <v>12347</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M20" t="inlineStr">
         <is>
           <t>ee_range</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>BB75</t>
-        </is>
-      </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>:(</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>JULIO Y RUBEN</t>
-        </is>
-      </c>
-      <c r="R20" t="n">
-        <v>6</v>
-      </c>
-      <c r="S20" t="n">
-        <v>6</v>
+          <t>description=- Component: TST Data
+- REPROG info: tbd</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TestData_11</t>
+          <t>TestData_10</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12349</v>
-      </c>
-      <c r="D21" t="inlineStr">
+        <v>12348</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>datablock</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>BB89</t>
-        </is>
-      </c>
-      <c r="P21" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>JEJ</t>
-        </is>
-      </c>
-      <c r="R21" t="n">
-        <v>5</v>
-      </c>
-      <c r="S21" t="n">
-        <v>9</v>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: t.b.d</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>TestData_11</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>12349</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: use case REPROG must be set</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>DUMMY_TestModuleCnt</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>31416</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>ee_erase</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>description=- Component: DUMMY
 - REPROG info: use case REPROG must not be set (data must not be changed after reprogramming)!
@@ -1672,79 +1608,32 @@
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>ASDFClockTower</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>111255</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>ee_datablock</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="O24" t="inlineStr">
         <is>
           <t>description=- Component: ASDF
 - REPROG info: use case REPROG must not be set.
 - REPROG info: In certain cases there are two comments of this type.
 There are also strings up to 160 characters per row, only on description fields and usually is not only one row. Like this example but a little bit longer.</t>
         </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>TestData_07</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>123456</v>
-      </c>
-      <c r="C24" t="n">
-        <v>91</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>ee_range</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>description=- Component: Test
-- REPROG info: To be evaluated.</t>
-        </is>
-      </c>
-      <c r="S24" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEAT] Al log de comparaciones se le agregaron los espacios para ver que elementos fueron eliminados del reporte previo y cuales elementos son totalmente nuevos en el reporte a generar
</commit_message>
<xml_diff>
--- a/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1432,18 +1432,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TestData_07</t>
+          <t>TestData_08</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12345</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
+        <v>12346</v>
+      </c>
+      <c r="C18" t="n">
+        <v>87</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1455,21 +1458,44 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>description=- Component: Test
-- REPROG info: To be evaluated.</t>
-        </is>
+          <t>HOLA</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>JULIO</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TestData_08</t>
+          <t>TestData_09</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12346</v>
-      </c>
-      <c r="I19" t="inlineStr">
+        <v>12347</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1479,23 +1505,54 @@
           <t>ee_range</t>
         </is>
       </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>BB96</t>
+        </is>
+      </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>description=- Component: TST Data
-- REPROG info: undefined</t>
-        </is>
+          <t>ADIOS</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>6</v>
+      </c>
+      <c r="R19" t="n">
+        <v>7</v>
+      </c>
+      <c r="S19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TestData_09</t>
+          <t>TestData_10</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12347</v>
-      </c>
-      <c r="G20" t="inlineStr">
+        <v>12348</v>
+      </c>
+      <c r="C20" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1505,21 +1562,51 @@
           <t>ee_range</t>
         </is>
       </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>BB75</t>
+        </is>
+      </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>description=- Component: TST Data
-- REPROG info: tbd</t>
-        </is>
+          <t>:(</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>JULIO Y RUBEN</t>
+        </is>
+      </c>
+      <c r="R20" t="n">
+        <v>6</v>
+      </c>
+      <c r="S20" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TestData_10</t>
+          <t>TestData_11</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12348</v>
+        <v>12349</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1533,34 +1620,37 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>ee_range</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>description=- Component: TST
-- REPROG info: t.b.d</t>
-        </is>
+          <t>datablock</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>BB89</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>JEJ</t>
+        </is>
+      </c>
+      <c r="R21" t="n">
+        <v>5</v>
+      </c>
+      <c r="S21" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TestData_11</t>
+          <t>DUMMY_TestModuleCnt</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>12349</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>31416</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1569,36 +1659,10 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>ee_range</t>
+          <t>ee_erase</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
-        <is>
-          <t>description=- Component: TST
-- REPROG info: use case REPROG must be set</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>DUMMY_TestModuleCnt</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>31416</v>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>ee_erase</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
         <is>
           <t>description=- Component: DUMMY
 - REPROG info: use case REPROG must not be set (data must not be changed after reprogramming)!
@@ -1608,32 +1672,79 @@
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
         <is>
           <t>ASDFClockTower</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B23" t="n">
         <v>111255</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
         <is>
           <t>ee_datablock</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>description=- Component: ASDF
 - REPROG info: use case REPROG must not be set.
 - REPROG info: In certain cases there are two comments of this type.
 There are also strings up to 160 characters per row, only on description fields and usually is not only one row. Like this example but a little bit longer.</t>
         </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TestData_07</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C24" t="n">
+        <v>91</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>description=- Component: Test
+- REPROG info: To be evaluated.</t>
+        </is>
+      </c>
+      <c r="S24" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEAT] project info se hizo opcional
</commit_message>
<xml_diff>
--- a/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
+++ b/ExternalFiles/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95650.xlsx
@@ -1432,21 +1432,18 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TestData_08</t>
+          <t>TestData_07</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>12346</v>
-      </c>
-      <c r="C18" t="n">
-        <v>87</v>
-      </c>
-      <c r="E18" t="inlineStr">
+        <v>12345</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1458,211 +1455,150 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>HOLA</t>
-        </is>
-      </c>
-      <c r="P18" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>JULIO</t>
-        </is>
-      </c>
-      <c r="S18" t="n">
-        <v>5</v>
+          <t>description=- Component: Test
+- REPROG info: To be evaluated.</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TestData_09</t>
+          <t>TestData_08</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12347</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" t="inlineStr">
+        <v>12346</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M19" t="inlineStr">
         <is>
           <t>ee_range</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>BB96</t>
-        </is>
-      </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>ADIOS</t>
-        </is>
-      </c>
-      <c r="P19" t="n">
-        <v>6</v>
-      </c>
-      <c r="R19" t="n">
-        <v>7</v>
-      </c>
-      <c r="S19" t="n">
-        <v>3</v>
+          <t>description=- Component: TST Data
+- REPROG info: undefined</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TestData_10</t>
+          <t>TestData_09</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12348</v>
-      </c>
-      <c r="C20" t="n">
-        <v>9</v>
-      </c>
-      <c r="D20" t="inlineStr">
+        <v>12347</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M20" t="inlineStr">
         <is>
           <t>ee_range</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>BB75</t>
-        </is>
-      </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>:(</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>JULIO Y RUBEN</t>
-        </is>
-      </c>
-      <c r="R20" t="n">
-        <v>6</v>
-      </c>
-      <c r="S20" t="n">
-        <v>6</v>
+          <t>description=- Component: TST Data
+- REPROG info: tbd</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TestData_11</t>
+          <t>TestData_10</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>12349</v>
-      </c>
-      <c r="D21" t="inlineStr">
+        <v>12348</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>datablock</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>BB89</t>
-        </is>
-      </c>
-      <c r="P21" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>JEJ</t>
-        </is>
-      </c>
-      <c r="R21" t="n">
-        <v>5</v>
-      </c>
-      <c r="S21" t="n">
-        <v>9</v>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: t.b.d</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>TestData_11</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>12349</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>ee_range</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>description=- Component: TST
+- REPROG info: use case REPROG must be set</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>DUMMY_TestModuleCnt</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B23" t="n">
         <v>31416</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>ee_erase</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>description=- Component: DUMMY
 - REPROG info: use case REPROG must not be set (data must not be changed after reprogramming)!
@@ -1672,79 +1608,32 @@
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>ASDFClockTower</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B24" t="n">
         <v>111255</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>ee_datablock</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="O24" t="inlineStr">
         <is>
           <t>description=- Component: ASDF
 - REPROG info: use case REPROG must not be set.
 - REPROG info: In certain cases there are two comments of this type.
 There are also strings up to 160 characters per row, only on description fields and usually is not only one row. Like this example but a little bit longer.</t>
         </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>TestData_07</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>123456</v>
-      </c>
-      <c r="C24" t="n">
-        <v>91</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>ee_range</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>description=- Component: Test
-- REPROG info: To be evaluated.</t>
-        </is>
-      </c>
-      <c r="S24" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>